<commit_message>
parametrized LCRLeader updated excel
</commit_message>
<xml_diff>
--- a/ModelTranslations/StatusTableOverview.xlsx
+++ b/ModelTranslations/StatusTableOverview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albin\Programmering\Exjobb\UML-To-Rebecca-Dataset\ModelTranslations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F8E457-569C-48CE-82C5-8831280469C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23C2218-C8C6-4AE2-8F46-CFD73A12DDAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -133,9 +133,6 @@
     <t>Message server first in transitions of PlantUML diagram</t>
   </si>
   <si>
-    <t>Send self loop in some states. Parametrize n parameter to only have one node class.</t>
-  </si>
-  <si>
     <t>Changes done</t>
   </si>
   <si>
@@ -146,6 +143,15 @@
   </si>
   <si>
     <t>Queue overflow, deadlock</t>
+  </si>
+  <si>
+    <t>Now only one node diagram. How to tell LLM how to initiate generic classes?</t>
+  </si>
+  <si>
+    <t>Turn train classes more generic? GPT sometimes creates duplicate classes.</t>
+  </si>
+  <si>
+    <t>Complete?</t>
   </si>
 </sst>
 </file>
@@ -1044,7 +1050,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,8 +1143,11 @@
       <c r="G3" s="3">
         <v>213</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>33</v>
+      <c r="H3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1192,16 +1201,16 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="H6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" t="s">
         <v>37</v>
-      </c>
-      <c r="I6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1220,11 +1229,11 @@
       <c r="E7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>32</v>
+      <c r="H7" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1264,7 +1273,7 @@
         <v>29</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
DoorController plantuml done needs to be reviewed
</commit_message>
<xml_diff>
--- a/ModelTranslations/StatusTableOverview.xlsx
+++ b/ModelTranslations/StatusTableOverview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albin\Programmering\Exjobb\UML-To-Rebecca-Dataset\ModelTranslations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albin\Programming\Exjobb\UML-To-Rebecca\ModelTranslations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23C2218-C8C6-4AE2-8F46-CFD73A12DDAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37C9DD2-2D2F-4622-8183-849D87579DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StatusTableOverview" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -100,9 +100,6 @@
     <t>Producer Consumer</t>
   </si>
   <si>
-    <t>OK, need potential properties</t>
-  </si>
-  <si>
     <t>OK, Starvation, Safety</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>Deadlock in diagram</t>
   </si>
   <si>
-    <t>Message server first in transitions of PlantUML diagram</t>
-  </si>
-  <si>
     <t>Changes done</t>
   </si>
   <si>
@@ -152,6 +146,15 @@
   </si>
   <si>
     <t>Complete?</t>
+  </si>
+  <si>
+    <t>https://rebeca-lang.org/assets/papers/2020/Towards-a-Verification-Driven-Iterative-Development-of-Cyber-Physical-System.pdf</t>
+  </si>
+  <si>
+    <t>OK, may need properties</t>
+  </si>
+  <si>
+    <t>Changed to be more alike our own process for translating diagrams.</t>
   </si>
 </sst>
 </file>
@@ -1049,24 +1052,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" customWidth="1"/>
-    <col min="9" max="9" width="83.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.73046875" customWidth="1"/>
+    <col min="3" max="3" width="11.265625" customWidth="1"/>
+    <col min="4" max="4" width="27.1328125" customWidth="1"/>
+    <col min="5" max="5" width="20.265625" customWidth="1"/>
+    <col min="6" max="6" width="17.3984375" customWidth="1"/>
+    <col min="7" max="7" width="22.3984375" customWidth="1"/>
+    <col min="8" max="8" width="24.86328125" customWidth="1"/>
+    <col min="9" max="9" width="83.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1089,13 +1092,13 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1106,10 +1109,10 @@
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="F2" s="3">
         <v>1472</v>
@@ -1118,10 +1121,10 @@
         <v>4533</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1132,10 +1135,10 @@
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3">
         <v>116</v>
@@ -1144,13 +1147,13 @@
         <v>213</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1161,19 +1164,19 @@
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1184,16 +1187,16 @@
         <v>15</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="E5" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="H5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1201,19 +1204,22 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1224,19 +1230,19 @@
         <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1247,16 +1253,16 @@
         <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="E8" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="H8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1267,31 +1273,42 @@
         <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="C10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="F10" s="3">
+        <v>471</v>
+      </c>
+      <c r="G10" s="3">
+        <v>537</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="I10" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1301,11 +1318,12 @@
     <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="C8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C10" r:id="rId6" xr:uid="{484A823D-CF21-4FAE-BB43-6CEC2939DC12}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated info on TicketService and S-Lab
</commit_message>
<xml_diff>
--- a/ModelTranslations/StatusTableOverview.xlsx
+++ b/ModelTranslations/StatusTableOverview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albin\Programming\Exjobb\UML-To-Rebecca\ModelTranslations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\UML-To-Rebecca-Dataset\ModelTranslations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E62782-AA63-4C5F-B4AD-2BFCAFC094AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C643F4-164F-475C-8652-6CC6C87CB2B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StatusTableOverview" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -124,9 +124,6 @@
     <t>Complete</t>
   </si>
   <si>
-    <t>Deadlock in diagram</t>
-  </si>
-  <si>
     <t>Changes done</t>
   </si>
   <si>
@@ -155,6 +152,15 @@
   </si>
   <si>
     <t>Queue overflow, increase to 6, deadlock. Adding else in giveMeNextProduce() solves deadlock (maybe).</t>
+  </si>
+  <si>
+    <t>Deadlock in diagram (more like Deadlock in code) Code needs to be fixed.</t>
+  </si>
+  <si>
+    <t>OK, but needs to be fixed</t>
+  </si>
+  <si>
+    <t>Waiting for review. But in main creates 2 Customers. The UML is more generic. No changed done to the code. How do GPT know that the constructors contains the variable "id" of the costumer?</t>
   </si>
 </sst>
 </file>
@@ -655,49 +661,49 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Dekorfärg1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Dekorfärg2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Dekorfärg3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Dekorfärg4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Dekorfärg5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Dekorfärg6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Dekorfärg1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Dekorfärg2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Dekorfärg3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Dekorfärg4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Dekorfärg5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Dekorfärg6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Dekorfärg1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Dekorfärg2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Dekorfärg3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Dekorfärg4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Dekorfärg5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Dekorfärg6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Anteckning" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Beräkning" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Bra" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Dekorfärg1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Dekorfärg2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Dekorfärg3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Dekorfärg4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Dekorfärg5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Dekorfärg6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Dålig" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Förklarande text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Hyperlänk" xfId="42" builtinId="8"/>
+    <cellStyle name="Indata" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Kontrollcell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Länkad cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Rubrik" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Rubrik 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Rubrik 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Rubrik 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Rubrik 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Summa" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Utdata" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Varningstext" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -721,12 +727,12 @@
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Rebeca Type"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Where" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Where"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Check in Afra"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Code Edits" dataCellStyle="Neutral"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Reached States"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Reached Transitions"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="PlantUML status" dataCellStyle="Bad"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="PlantUML status"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -734,7 +740,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1053,23 +1059,23 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="22.73046875" customWidth="1"/>
-    <col min="3" max="3" width="11.265625" customWidth="1"/>
-    <col min="4" max="4" width="27.1328125" customWidth="1"/>
-    <col min="5" max="5" width="20.265625" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" customWidth="1"/>
-    <col min="7" max="7" width="22.3984375" customWidth="1"/>
-    <col min="8" max="8" width="24.86328125" customWidth="1"/>
-    <col min="9" max="9" width="83.265625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" customWidth="1"/>
+    <col min="9" max="9" width="83.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1098,7 +1104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1124,7 +1130,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1147,13 +1153,13 @@
         <v>213</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1163,20 +1169,20 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>31</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1196,7 +1202,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1204,22 +1210,22 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1236,13 +1242,13 @@
         <v>28</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1262,7 +1268,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1273,16 +1279,25 @@
         <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="F9" s="3">
+        <v>699</v>
+      </c>
+      <c r="G9" s="3">
+        <v>827</v>
+      </c>
       <c r="H9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="I9" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1290,10 +1305,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>28</v>
@@ -1305,10 +1320,10 @@
         <v>537</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Zero-Shot attempt of train bridge controller
</commit_message>
<xml_diff>
--- a/ModelTranslations/StatusTableOverview.xlsx
+++ b/ModelTranslations/StatusTableOverview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\UML-To-Rebecca-Dataset\ModelTranslations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albin\Programming\Exjobb\UML-To-Rebecca\ModelTranslations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C643F4-164F-475C-8652-6CC6C87CB2B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE0E10D-5C85-4773-AB68-FC3DE8D14C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StatusTableOverview" sheetId="1" r:id="rId1"/>
@@ -661,49 +661,49 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20 % - Dekorfärg1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Dekorfärg2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Dekorfärg3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Dekorfärg4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Dekorfärg5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Dekorfärg6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Dekorfärg1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Dekorfärg2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Dekorfärg3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Dekorfärg4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Dekorfärg5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Dekorfärg6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Dekorfärg1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Dekorfärg2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Dekorfärg3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Dekorfärg4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Dekorfärg5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Dekorfärg6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Anteckning" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Beräkning" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Bra" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Dekorfärg1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Dekorfärg2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Dekorfärg3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Dekorfärg4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Dekorfärg5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Dekorfärg6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Dålig" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Förklarande text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Hyperlänk" xfId="42" builtinId="8"/>
-    <cellStyle name="Indata" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Kontrollcell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Länkad cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Rubrik" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Rubrik 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Rubrik 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Rubrik 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Rubrik 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Summa" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Utdata" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Varningstext" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -740,7 +740,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1059,23 +1059,23 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" customWidth="1"/>
-    <col min="9" max="9" width="83.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.73046875" customWidth="1"/>
+    <col min="3" max="3" width="11.265625" customWidth="1"/>
+    <col min="4" max="4" width="27.1328125" customWidth="1"/>
+    <col min="5" max="5" width="20.265625" customWidth="1"/>
+    <col min="6" max="6" width="17.3984375" customWidth="1"/>
+    <col min="7" max="7" width="22.3984375" customWidth="1"/>
+    <col min="8" max="8" width="24.86328125" customWidth="1"/>
+    <col min="9" max="9" width="83.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Code edit for DiningPhilosophers.rebeca
</commit_message>
<xml_diff>
--- a/ModelTranslations/StatusTableOverview.xlsx
+++ b/ModelTranslations/StatusTableOverview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albin\Programming\Exjobb\UML-To-Rebecca\ModelTranslations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE0E10D-5C85-4773-AB68-FC3DE8D14C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5974237-7CDD-44D0-8DDE-98A4FAFEF241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>Waiting for review. But in main creates 2 Customers. The UML is more generic. No changed done to the code. How do GPT know that the constructors contains the variable "id" of the costumer?</t>
+  </si>
+  <si>
+    <t>msgsrv -&gt; constructor, removed comments</t>
   </si>
 </sst>
 </file>
@@ -1059,7 +1062,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1117,8 +1120,8 @@
       <c r="D2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>28</v>
+      <c r="E2" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="F2" s="3">
         <v>1472</v>

</xml_diff>

<commit_message>
Code edits confirmed for TrainBridgeController.rebeca
</commit_message>
<xml_diff>
--- a/ModelTranslations/StatusTableOverview.xlsx
+++ b/ModelTranslations/StatusTableOverview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albin\Programming\Exjobb\UML-To-Rebecca\ModelTranslations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5974237-7CDD-44D0-8DDE-98A4FAFEF241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A894300-C24D-4DC0-8F01-1BF64F5CCB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>msgsrv -&gt; constructor, removed comments</t>
+  </si>
+  <si>
+    <t>removed comments</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1065,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1123,10 +1126,10 @@
       <c r="E2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>1472</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>4533</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -1146,13 +1149,13 @@
       <c r="D3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="E3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="2">
         <v>116</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>213</v>
       </c>
       <c r="H3" s="3" t="s">

</xml_diff>

<commit_message>
Code edit confirmed for LCRLeader.rebeca
</commit_message>
<xml_diff>
--- a/ModelTranslations/StatusTableOverview.xlsx
+++ b/ModelTranslations/StatusTableOverview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albin\Programming\Exjobb\UML-To-Rebecca\ModelTranslations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A894300-C24D-4DC0-8F01-1BF64F5CCB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345DA5E6-B75B-4271-B6E0-67487F9E4232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,9 +103,6 @@
     <t>OK, Starvation, Safety</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
     <t>OK, Safety, Deadlock, Starvation</t>
   </si>
   <si>
@@ -167,6 +164,9 @@
   </si>
   <si>
     <t>removed comments</t>
+  </si>
+  <si>
+    <t>OK, Progress</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1065,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1104,7 +1104,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -1121,10 +1121,10 @@
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F2" s="2">
         <v>1472</v>
@@ -1133,7 +1133,7 @@
         <v>4533</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
@@ -1150,7 +1150,7 @@
         <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" s="2">
         <v>116</v>
@@ -1159,10 +1159,10 @@
         <v>213</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
@@ -1176,16 +1176,16 @@
         <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -1199,13 +1199,13 @@
         <v>15</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
@@ -1216,19 +1216,19 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
@@ -1242,16 +1242,22 @@
         <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="2">
         <v>28</v>
       </c>
+      <c r="G7" s="2">
+        <v>49</v>
+      </c>
       <c r="H7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
@@ -1265,13 +1271,13 @@
         <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
@@ -1285,10 +1291,10 @@
         <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="3">
         <v>699</v>
@@ -1297,10 +1303,10 @@
         <v>827</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
@@ -1311,13 +1317,13 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="3">
         <v>471</v>
@@ -1326,10 +1332,10 @@
         <v>537</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code edit for ProducerConsumer.rebeca
</commit_message>
<xml_diff>
--- a/ModelTranslations/StatusTableOverview.xlsx
+++ b/ModelTranslations/StatusTableOverview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albin\Programming\Exjobb\UML-To-Rebecca\ModelTranslations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345DA5E6-B75B-4271-B6E0-67487F9E4232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7773B6-3568-43B9-A506-EA0630254AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -127,9 +127,6 @@
     <t>https://rebeca-lang.org/allprojects/SysfierExamples/ProducerConsumer</t>
   </si>
   <si>
-    <t>Queue overflow, deadlock</t>
-  </si>
-  <si>
     <t>Now only one node diagram. How to tell LLM how to initiate generic classes?</t>
   </si>
   <si>
@@ -167,6 +164,12 @@
   </si>
   <si>
     <t>OK, Progress</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>msgsrv -&gt; constructor, added else in giveNextProduce()</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +1127,7 @@
         <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F2" s="2">
         <v>1472</v>
@@ -1150,7 +1153,7 @@
         <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" s="2">
         <v>116</v>
@@ -1159,10 +1162,10 @@
         <v>213</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
@@ -1176,7 +1179,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>27</v>
@@ -1185,7 +1188,7 @@
         <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -1218,17 +1221,23 @@
       <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>27</v>
+      <c r="D6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="2">
+        <v>161</v>
+      </c>
+      <c r="G6" s="2">
+        <v>275</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
@@ -1242,10 +1251,10 @@
         <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" s="2">
         <v>28</v>
@@ -1257,7 +1266,7 @@
         <v>32</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
@@ -1291,7 +1300,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>27</v>
@@ -1306,7 +1315,7 @@
         <v>32</v>
       </c>
       <c r="I9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
@@ -1317,10 +1326,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>27</v>
@@ -1335,7 +1344,7 @@
         <v>32</v>
       </c>
       <c r="I10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed comments from DoorController.rebeca
</commit_message>
<xml_diff>
--- a/ModelTranslations/StatusTableOverview.xlsx
+++ b/ModelTranslations/StatusTableOverview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albin\Programming\Exjobb\UML-To-Rebecca\ModelTranslations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7773B6-3568-43B9-A506-EA0630254AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE1483D-34F4-4600-8CD0-F1480FEC3EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1068,7 +1068,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1331,8 +1331,8 @@
       <c r="D10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>27</v>
+      <c r="E10" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="F10" s="3">
         <v>471</v>

</xml_diff>

<commit_message>
readme and excel update
</commit_message>
<xml_diff>
--- a/ModelTranslations/StatusTableOverview.xlsx
+++ b/ModelTranslations/StatusTableOverview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albin\Programming\Exjobb\UML-To-Rebecca\ModelTranslations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE1483D-34F4-4600-8CD0-F1480FEC3EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFB55E1-F6C8-4AFD-9D04-75485695947F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>Turn train classes more generic? GPT sometimes creates duplicate classes.</t>
-  </si>
-  <si>
-    <t>Complete?</t>
   </si>
   <si>
     <t>https://rebeca-lang.org/assets/papers/2020/Towards-a-Verification-Driven-Iterative-Development-of-Cyber-Physical-System.pdf</t>
@@ -1067,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1127,7 +1124,7 @@
         <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="2">
         <v>1472</v>
@@ -1153,7 +1150,7 @@
         <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3" s="2">
         <v>116</v>
@@ -1161,8 +1158,8 @@
       <c r="G3" s="2">
         <v>213</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>36</v>
+      <c r="H3" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="I3" t="s">
         <v>35</v>
@@ -1179,7 +1176,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>27</v>
@@ -1188,7 +1185,7 @@
         <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -1222,10 +1219,10 @@
         <v>33</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="F6" s="2">
         <v>161</v>
@@ -1237,7 +1234,7 @@
         <v>32</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
@@ -1251,10 +1248,10 @@
         <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="2">
         <v>28</v>
@@ -1300,7 +1297,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>27</v>
@@ -1311,11 +1308,11 @@
       <c r="G9" s="3">
         <v>827</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>32</v>
+      <c r="H9" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="I9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
@@ -1326,13 +1323,13 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="3">
         <v>471</v>
@@ -1344,7 +1341,7 @@
         <v>32</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sender Receiver wrong spelling
</commit_message>
<xml_diff>
--- a/ModelTranslations/StatusTableOverview.xlsx
+++ b/ModelTranslations/StatusTableOverview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albin\Programming\Exjobb\UML-To-Rebecca\ModelTranslations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFB55E1-F6C8-4AFD-9D04-75485695947F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F704A52A-FCC0-4421-953B-EE010501F309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StatusTableOverview" sheetId="1" r:id="rId1"/>
@@ -94,9 +94,6 @@
     <t>Commit Problem</t>
   </si>
   <si>
-    <t>Sender Reciever</t>
-  </si>
-  <si>
     <t>Producer Consumer</t>
   </si>
   <si>
@@ -167,6 +164,9 @@
   </si>
   <si>
     <t>msgsrv -&gt; constructor, added else in giveNextProduce()</t>
+  </si>
+  <si>
+    <t>Sender Receiver</t>
   </si>
 </sst>
 </file>
@@ -728,7 +728,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I10" totalsRowShown="0">
   <autoFilter ref="A1:I10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I10">
-    <sortCondition ref="H1:H10"/>
+    <sortCondition ref="A1:A10"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
@@ -1064,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1104,7 +1104,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -1112,126 +1112,126 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1472</v>
-      </c>
-      <c r="G2" s="2">
-        <v>4533</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>31</v>
+      <c r="H2" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F3" s="2">
-        <v>116</v>
+        <v>1472</v>
       </c>
       <c r="G3" s="2">
-        <v>213</v>
+        <v>4533</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="2">
+        <v>161</v>
+      </c>
+      <c r="G4" s="2">
+        <v>275</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="2">
         <v>28</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>30</v>
+      <c r="G5" s="2">
+        <v>49</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="2">
-        <v>161</v>
-      </c>
-      <c r="G6" s="2">
-        <v>275</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>32</v>
+        <v>11</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="I6" t="s">
         <v>39</v>
@@ -1239,119 +1239,119 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="2">
-        <v>28</v>
-      </c>
-      <c r="G7" s="2">
-        <v>49</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" t="s">
-        <v>34</v>
+        <v>16</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="3">
+        <v>699</v>
+      </c>
+      <c r="G8" s="3">
+        <v>827</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>30</v>
+      </c>
+      <c r="I8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
-        <v>11</v>
+      <c r="C9" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="3">
+        <v>471</v>
+      </c>
+      <c r="G9" s="3">
+        <v>537</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" t="s">
         <v>37</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="3">
-        <v>699</v>
-      </c>
-      <c r="G9" s="3">
-        <v>827</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>37</v>
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="3">
-        <v>471</v>
-      </c>
-      <c r="G10" s="3">
-        <v>537</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>32</v>
+        <v>43</v>
+      </c>
+      <c r="F10" s="2">
+        <v>116</v>
+      </c>
+      <c r="G10" s="2">
+        <v>213</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="I10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C10" r:id="rId6" xr:uid="{484A823D-CF21-4FAE-BB43-6CEC2939DC12}"/>
+    <hyperlink ref="C10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C9" r:id="rId6" xr:uid="{484A823D-CF21-4FAE-BB43-6CEC2939DC12}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>

</xml_diff>

<commit_message>
Added yarn and spanning tree examples
</commit_message>
<xml_diff>
--- a/ModelTranslations/StatusTableOverview.xlsx
+++ b/ModelTranslations/StatusTableOverview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albin\Programming\Exjobb\UML-To-Rebecca\ModelTranslations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F704A52A-FCC0-4421-953B-EE010501F309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983666C5-2FAF-4816-B230-842E546897E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StatusTableOverview" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -167,6 +167,18 @@
   </si>
   <si>
     <t>Sender Receiver</t>
+  </si>
+  <si>
+    <t>https://rebeca-lang.org/allprojects/SysfierExamples/SpanningTreeProtocol</t>
+  </si>
+  <si>
+    <t>Spanning Tree Protocol</t>
+  </si>
+  <si>
+    <t>https://rebeca-lang.org/Rebeca</t>
+  </si>
+  <si>
+    <t>Hadoop Yarn Schedule</t>
   </si>
 </sst>
 </file>
@@ -725,8 +737,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I10" totalsRowShown="0">
-  <autoFilter ref="A1:I10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I12" totalsRowShown="0">
+  <autoFilter ref="A1:I12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I10">
     <sortCondition ref="A1:A10"/>
   </sortState>
@@ -1062,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1344,6 +1356,34 @@
         <v>34</v>
       </c>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -1352,11 +1392,13 @@
     <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="C7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="C9" r:id="rId6" xr:uid="{484A823D-CF21-4FAE-BB43-6CEC2939DC12}"/>
+    <hyperlink ref="C12" r:id="rId7" xr:uid="{B2B435D9-EF4A-45F4-BBB0-E85D1C15997F}"/>
+    <hyperlink ref="C11" r:id="rId8" xr:uid="{34D8959F-D557-4050-8885-E58DEE55CD44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>